<commit_message>
Updated specification to use currencies for all currency fields, and tests to use a Money class that wraps BigDecimal
</commit_message>
<xml_diff>
--- a/src/test/resources/org/concordion/ext/excel/tutorial/FirstExcelTutorial.xlsx
+++ b/src/test/resources/org/concordion/ext/excel/tutorial/FirstExcelTutorial.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="12180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Taxi Fare Examples" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="Flat_Rate">'Taxi Fare Examples'!$B$3</definedName>
     <definedName name="LowMiles">'Taxi Fare Examples'!$D$4</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -247,8 +247,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -316,15 +317,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -339,19 +341,24 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="[$£-809]#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -363,13 +370,13 @@
     <tableColumn id="5" name="Flat Fee" dataDxfId="3">
       <calculatedColumnFormula>Flat_Rate</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="First Cost" dataDxfId="2">
+    <tableColumn id="3" name="First Cost" dataDxfId="1">
       <calculatedColumnFormula>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Second Cost" dataDxfId="1">
+    <tableColumn id="2" name="Second Cost" dataDxfId="0">
       <calculatedColumnFormula>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Total Cost" dataDxfId="0">
+    <tableColumn id="4" name="Total Cost" dataDxfId="2">
       <calculatedColumnFormula>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -702,24 +709,24 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -727,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -744,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -755,19 +762,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -784,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -792,20 +799,20 @@
         <f t="shared" ref="B10:B16" si="0">Flat_Rate</f>
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>0</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -813,20 +820,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>2.8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -834,20 +841,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -855,20 +862,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>5.3999999999999995</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>6.3999999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -876,20 +883,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="6">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="6">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>0.6</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="6">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>7.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>20</v>
       </c>
@@ -897,20 +904,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="6">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>6</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="6">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>25</v>
       </c>
@@ -918,15 +925,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="6">
         <f>MIN(LowMiles,Table1[[#This Row],[Distance]])*CostPerMile</f>
         <v>6</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="6">
         <f>MAX(0, Table1[[#This Row],[Distance]]-LowMiles)*CostPerMileHigh</f>
         <v>4.5</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <f>Table1[[#This Row],[Flat Fee]]+Table1[[#This Row],[First Cost]]+Table1[[#This Row],[Second Cost]]</f>
         <v>11.5</v>
       </c>
@@ -936,10 +943,10 @@
     <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>